<commit_message>
feat: complete waiting list
</commit_message>
<xml_diff>
--- a/GoodOldGoods_Data.xlsx
+++ b/GoodOldGoods_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\filipe\opl\GoodOldGoods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF62B559-596E-4EC3-9C32-DB13E4106D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A18CF4-2707-40FB-9F50-F35C8A0150D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{51444302-351F-4C6A-9509-FCF90DE566BE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="2" xr2:uid="{51444302-351F-4C6A-9509-FCF90DE566BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <definedName name="Days">Table1[[#Headers],[Day 1]:[Day 9]]</definedName>
     <definedName name="LanguageSkillsMatch">'Table 4'!$E$5:$E$38</definedName>
     <definedName name="PositionMatch">'Table 4'!$C$5:$C$38</definedName>
-    <definedName name="Positions">'Table 1'!$B$5:$B$39</definedName>
+    <definedName name="Positions">'Table 1'!$B$5:$B$38</definedName>
     <definedName name="PresentationSkillsMatch">'Table 4'!$D$5:$D$38</definedName>
     <definedName name="Requirements">'Table 1'!$O$5:$W$39</definedName>
   </definedNames>
@@ -1333,7 +1333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1367,26 +1367,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="6"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1460,11 +1440,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2899,8 +2879,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0934F15-1586-43ED-9E4B-C49A52B31BCE}">
   <dimension ref="B2:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:L5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -17343,8 +17323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{804420F3-B227-496E-9076-6CB8E80B7648}">
   <dimension ref="B2:V334"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17395,6 +17375,7 @@
       <c r="Q3" s="24"/>
       <c r="R3" s="24"/>
       <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
     </row>
     <row r="4" spans="2:22" s="15" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
       <c r="B4" s="16" t="s">
@@ -38913,7 +38894,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D3:S3"/>
+    <mergeCell ref="D3:T3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -38926,8 +38907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7371474-674C-4309-8ADA-EB747E0F244C}">
   <dimension ref="B4:E39"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>